<commit_message>
Update file paths in run.py
</commit_message>
<xml_diff>
--- a/api/test.xlsx
+++ b/api/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK38"/>
+  <dimension ref="A1:AK39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -626,7 +626,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -635,28 +635,28 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>382.48</v>
+        <v>1865.08</v>
       </c>
       <c r="F2" t="n">
-        <v>286</v>
+        <v>1764</v>
       </c>
       <c r="G2" t="n">
-        <v>20378</v>
+        <v>81700</v>
       </c>
       <c r="H2" t="n">
-        <v>79861</v>
+        <v>241426</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>96.48</v>
+        <v>101.08</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>286</v>
+        <v>1764</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -668,28 +668,28 @@
         <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>79861</v>
+        <v>241426</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>106.24</v>
+        <v>518.08</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>26.8</v>
+        <v>28.08</v>
       </c>
       <c r="U2" t="n">
         <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>79.44</v>
+        <v>490</v>
       </c>
       <c r="W2" t="n">
-        <v>79.44</v>
+        <v>490</v>
       </c>
       <c r="X2" t="n">
         <v>0</v>
@@ -698,28 +698,28 @@
         <v>0</v>
       </c>
       <c r="Z2" t="n">
-        <v>223.66</v>
+        <v>891.6799999999999</v>
       </c>
       <c r="AA2" t="n">
-        <v>79.86</v>
+        <v>241.43</v>
       </c>
       <c r="AB2" t="n">
         <v>0</v>
       </c>
       <c r="AC2" t="n">
-        <v>79.86</v>
+        <v>241.43</v>
       </c>
       <c r="AD2" t="n">
         <v>0</v>
       </c>
       <c r="AE2" t="n">
-        <v>57.09</v>
+        <v>68.20999999999999</v>
       </c>
       <c r="AF2" t="n">
         <v>0</v>
       </c>
       <c r="AG2" t="n">
-        <v>42.91</v>
+        <v>31.79</v>
       </c>
       <c r="AH2" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -762,28 +762,28 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>230.08</v>
+        <v>1335.35</v>
       </c>
       <c r="F3" t="n">
-        <v>155</v>
+        <v>1197</v>
       </c>
       <c r="G3" t="n">
-        <v>10862</v>
+        <v>48739</v>
       </c>
       <c r="H3" t="n">
-        <v>32502</v>
+        <v>88968</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>75.08</v>
+        <v>138.35</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>155</v>
+        <v>1197</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -795,28 +795,28 @@
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>32502</v>
+        <v>88968</v>
       </c>
       <c r="Q3" t="n">
         <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>63.91</v>
+        <v>370.93</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>20.86</v>
+        <v>38.43</v>
       </c>
       <c r="U3" t="n">
         <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>43.06</v>
+        <v>332.5</v>
       </c>
       <c r="W3" t="n">
-        <v>43.06</v>
+        <v>332.5</v>
       </c>
       <c r="X3" t="n">
         <v>0</v>
@@ -825,28 +825,28 @@
         <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>119.21</v>
+        <v>531.9400000000001</v>
       </c>
       <c r="AA3" t="n">
-        <v>32.5</v>
+        <v>88.97</v>
       </c>
       <c r="AB3" t="n">
         <v>0</v>
       </c>
       <c r="AC3" t="n">
-        <v>32.5</v>
+        <v>88.97</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
       </c>
       <c r="AE3" t="n">
-        <v>66.29000000000001</v>
+        <v>80.65000000000001</v>
       </c>
       <c r="AF3" t="n">
         <v>0</v>
       </c>
       <c r="AG3" t="n">
-        <v>33.71</v>
+        <v>19.35</v>
       </c>
       <c r="AH3" t="inlineStr">
         <is>
@@ -880,7 +880,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -889,28 +889,28 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1396.51</v>
+        <v>6509.95</v>
       </c>
       <c r="F4" t="n">
-        <v>1032.01</v>
+        <v>5784.67</v>
       </c>
       <c r="G4" t="n">
-        <v>73159</v>
+        <v>291791</v>
       </c>
       <c r="H4" t="n">
-        <v>246931</v>
+        <v>836364</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>364.5</v>
+        <v>725.28</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>1032.01</v>
+        <v>5784.67</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -922,28 +922,28 @@
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>246931</v>
+        <v>836364</v>
       </c>
       <c r="Q4" t="n">
         <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>387.92</v>
+        <v>1808.32</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>101.25</v>
+        <v>201.47</v>
       </c>
       <c r="U4" t="n">
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>286.67</v>
+        <v>1606.85</v>
       </c>
       <c r="W4" t="n">
-        <v>286.67</v>
+        <v>1606.85</v>
       </c>
       <c r="X4" t="n">
         <v>0</v>
@@ -952,28 +952,28 @@
         <v>0</v>
       </c>
       <c r="Z4" t="n">
-        <v>802.9400000000001</v>
+        <v>3184.64</v>
       </c>
       <c r="AA4" t="n">
-        <v>246.93</v>
+        <v>836.36</v>
       </c>
       <c r="AB4" t="n">
         <v>0</v>
       </c>
       <c r="AC4" t="n">
-        <v>246.93</v>
+        <v>836.36</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
       </c>
       <c r="AE4" t="n">
-        <v>61.1</v>
+        <v>68.38</v>
       </c>
       <c r="AF4" t="n">
         <v>0</v>
       </c>
       <c r="AG4" t="n">
-        <v>38.9</v>
+        <v>31.62</v>
       </c>
       <c r="AH4" t="inlineStr">
         <is>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1016,13 +1016,13 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>72.98</v>
+        <v>667.17</v>
       </c>
       <c r="F5" t="n">
-        <v>59.73</v>
+        <v>607.64</v>
       </c>
       <c r="G5" t="n">
-        <v>1718.55</v>
+        <v>19476</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -1031,13 +1031,13 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>13.25</v>
+        <v>59.53</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>59.73</v>
+        <v>607.64</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -1055,22 +1055,22 @@
         <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>20.27</v>
+        <v>185.32</v>
       </c>
       <c r="S5" t="n">
         <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>3.68</v>
+        <v>16.54</v>
       </c>
       <c r="U5" t="n">
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>16.59</v>
+        <v>168.79</v>
       </c>
       <c r="W5" t="n">
-        <v>16.59</v>
+        <v>168.79</v>
       </c>
       <c r="X5" t="n">
         <v>0</v>
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>18.86</v>
+        <v>212.56</v>
       </c>
       <c r="AA5" t="n">
         <v>0</v>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1143,28 +1143,28 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1029.71</v>
+        <v>5643.39</v>
       </c>
       <c r="F6" t="n">
-        <v>763</v>
+        <v>5459</v>
       </c>
       <c r="G6" t="n">
-        <v>62087</v>
+        <v>274621</v>
       </c>
       <c r="H6" t="n">
-        <v>233854</v>
+        <v>770267</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>266.71</v>
+        <v>184.39</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>763</v>
+        <v>5459</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
@@ -1176,28 +1176,28 @@
         <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>233854</v>
+        <v>770267</v>
       </c>
       <c r="Q6" t="n">
         <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>286.03</v>
+        <v>1567.61</v>
       </c>
       <c r="S6" t="n">
         <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>74.08</v>
+        <v>51.22</v>
       </c>
       <c r="U6" t="n">
         <v>0</v>
       </c>
       <c r="V6" t="n">
-        <v>211.94</v>
+        <v>1516.39</v>
       </c>
       <c r="W6" t="n">
-        <v>211.94</v>
+        <v>1516.39</v>
       </c>
       <c r="X6" t="n">
         <v>0</v>
@@ -1206,28 +1206,28 @@
         <v>0</v>
       </c>
       <c r="Z6" t="n">
-        <v>681.42</v>
+        <v>2993.37</v>
       </c>
       <c r="AA6" t="n">
-        <v>233.85</v>
+        <v>770.27</v>
       </c>
       <c r="AB6" t="n">
         <v>0</v>
       </c>
       <c r="AC6" t="n">
-        <v>233.85</v>
+        <v>770.27</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
       </c>
       <c r="AE6" t="n">
-        <v>55.02</v>
+        <v>67.05</v>
       </c>
       <c r="AF6" t="n">
         <v>0</v>
       </c>
       <c r="AG6" t="n">
-        <v>44.98</v>
+        <v>32.95</v>
       </c>
       <c r="AH6" t="inlineStr">
         <is>
@@ -1256,42 +1256,42 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">ČEZ Energo, s.r.o., U Řezné 367, Železná Ruda </t>
+          <t>ČEZ Energo, s.r.o., Na Bradle  969, Světlá nad Sázavou</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>27ZG300Z0249899N</t>
+          <t>27ZG500Z0341998U</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>166.23</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>156</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>1513</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>2322</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>10.23</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>156</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -1303,28 +1303,28 @@
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>2322</v>
+        <v>0</v>
       </c>
       <c r="Q7" t="n">
         <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>46.17</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
         <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>2.84</v>
+        <v>0</v>
       </c>
       <c r="U7" t="n">
         <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>43.33</v>
+        <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>43.33</v>
+        <v>0</v>
       </c>
       <c r="X7" t="n">
         <v>0</v>
@@ -1333,28 +1333,28 @@
         <v>0</v>
       </c>
       <c r="Z7" t="n">
-        <v>16.57</v>
+        <v>0</v>
       </c>
       <c r="AA7" t="n">
-        <v>2.32</v>
+        <v>0</v>
       </c>
       <c r="AB7" t="n">
         <v>0</v>
       </c>
       <c r="AC7" t="n">
-        <v>2.32</v>
+        <v>0</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
       </c>
       <c r="AE7" t="n">
-        <v>95.20999999999999</v>
+        <v>0</v>
       </c>
       <c r="AF7" t="n">
         <v>0</v>
       </c>
       <c r="AG7" t="n">
-        <v>4.79</v>
+        <v>0</v>
       </c>
       <c r="AH7" t="inlineStr">
         <is>
@@ -1383,42 +1383,42 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">ČEZ Energo, s.r.o., Šumavská 112, Železná Ruda </t>
+          <t xml:space="preserve">ČEZ Energo, s.r.o., U Řezné 367, Železná Ruda </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>27ZG300Z0249900R</t>
+          <t>27ZG300Z0249899N</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>80.93000000000001</v>
+        <v>780.23</v>
       </c>
       <c r="F8" t="n">
-        <v>63</v>
+        <v>721</v>
       </c>
       <c r="G8" t="n">
-        <v>2401</v>
+        <v>1457</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>2430</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>17.93</v>
+        <v>59.23</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>63</v>
+        <v>721</v>
       </c>
       <c r="M8" t="n">
         <v>0</v>
@@ -1430,28 +1430,28 @@
         <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>2430</v>
       </c>
       <c r="Q8" t="n">
         <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>22.48</v>
+        <v>216.73</v>
       </c>
       <c r="S8" t="n">
         <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>4.98</v>
+        <v>16.45</v>
       </c>
       <c r="U8" t="n">
         <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>17.5</v>
+        <v>200.28</v>
       </c>
       <c r="W8" t="n">
-        <v>17.5</v>
+        <v>200.28</v>
       </c>
       <c r="X8" t="n">
         <v>0</v>
@@ -1460,39 +1460,39 @@
         <v>0</v>
       </c>
       <c r="Z8" t="n">
-        <v>26.29</v>
+        <v>15.93</v>
       </c>
       <c r="AA8" t="n">
-        <v>0</v>
+        <v>2.43</v>
       </c>
       <c r="AB8" t="n">
         <v>0</v>
       </c>
       <c r="AC8" t="n">
-        <v>0</v>
+        <v>2.43</v>
       </c>
       <c r="AD8" t="n">
         <v>0</v>
       </c>
       <c r="AE8" t="n">
-        <v>100</v>
+        <v>98.89</v>
       </c>
       <c r="AF8" t="n">
         <v>0</v>
       </c>
       <c r="AG8" t="n">
-        <v>0</v>
+        <v>1.11</v>
       </c>
       <c r="AH8" t="inlineStr">
         <is>
+          <t>ANO</t>
+        </is>
+      </c>
+      <c r="AI8" t="inlineStr">
+        <is>
           <t>NE</t>
         </is>
       </c>
-      <c r="AI8" t="inlineStr">
-        <is>
-          <t>NE</t>
-        </is>
-      </c>
       <c r="AJ8" t="inlineStr">
         <is>
           <t>ANO</t>
@@ -1500,7 +1500,7 @@
       </c>
       <c r="AK8" t="inlineStr">
         <is>
-          <t>DK</t>
+          <t>O</t>
         </is>
       </c>
     </row>
@@ -1510,27 +1510,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Na Výsluní 719, Zruč nad Sázavou</t>
+          <t xml:space="preserve">ČEZ Energo, s.r.o., Šumavská 112, Železná Ruda </t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>27ZG200Z0236068P</t>
+          <t>27ZG300Z0249900R</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>332.65</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>301</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>9884</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1539,13 +1539,13 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>31.65</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>301</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
@@ -1563,22 +1563,22 @@
         <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>0</v>
+        <v>92.40000000000001</v>
       </c>
       <c r="S9" t="n">
         <v>0</v>
       </c>
       <c r="T9" t="n">
-        <v>0</v>
+        <v>8.789999999999999</v>
       </c>
       <c r="U9" t="n">
         <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>0</v>
+        <v>83.61</v>
       </c>
       <c r="W9" t="n">
-        <v>0</v>
+        <v>83.61</v>
       </c>
       <c r="X9" t="n">
         <v>0</v>
@@ -1587,7 +1587,7 @@
         <v>0</v>
       </c>
       <c r="Z9" t="n">
-        <v>0</v>
+        <v>108.07</v>
       </c>
       <c r="AA9" t="n">
         <v>0</v>
@@ -1602,7 +1602,7 @@
         <v>0</v>
       </c>
       <c r="AE9" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AF9" t="n">
         <v>0</v>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="AK9" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>DK</t>
         </is>
       </c>
     </row>
@@ -1637,30 +1637,30 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Na Výsluní  719, Zruč nad Sázavou</t>
+          <t>ČEZ Energo, s.r.o., Na Výsluní 719, Zruč nad Sázavou</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>27ZG200Z0256193A</t>
+          <t>27ZG200Z0236068P</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>918.98</v>
+        <v>29</v>
       </c>
       <c r="F10" t="n">
-        <v>918.98</v>
+        <v>29</v>
       </c>
       <c r="G10" t="n">
-        <v>47684</v>
+        <v>893.45</v>
       </c>
       <c r="H10" t="n">
-        <v>194117.42</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -1672,7 +1672,7 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>918.98</v>
+        <v>29</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
@@ -1684,13 +1684,13 @@
         <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>194117.42</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="n">
         <v>0</v>
       </c>
       <c r="R10" t="n">
-        <v>255.27</v>
+        <v>8.06</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -1702,10 +1702,10 @@
         <v>0</v>
       </c>
       <c r="V10" t="n">
-        <v>255.27</v>
+        <v>8.06</v>
       </c>
       <c r="W10" t="n">
-        <v>255.27</v>
+        <v>8.06</v>
       </c>
       <c r="X10" t="n">
         <v>0</v>
@@ -1714,32 +1714,32 @@
         <v>0</v>
       </c>
       <c r="Z10" t="n">
-        <v>523.71</v>
+        <v>9.779999999999999</v>
       </c>
       <c r="AA10" t="n">
-        <v>194.12</v>
+        <v>0</v>
       </c>
       <c r="AB10" t="n">
         <v>0</v>
       </c>
       <c r="AC10" t="n">
-        <v>194.12</v>
+        <v>0</v>
       </c>
       <c r="AD10" t="n">
         <v>0</v>
       </c>
       <c r="AE10" t="n">
-        <v>56.8</v>
+        <v>100</v>
       </c>
       <c r="AF10" t="n">
         <v>0</v>
       </c>
       <c r="AG10" t="n">
-        <v>43.2</v>
+        <v>0</v>
       </c>
       <c r="AH10" t="inlineStr">
         <is>
-          <t>ANO</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="AI10" t="inlineStr">
@@ -1764,30 +1764,30 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Sídliště 9890, Smiřice</t>
+          <t>ČEZ Energo, s.r.o., Na Výsluní  719, Zruč nad Sázavou</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>27ZG500Z02916194</t>
+          <t>27ZG200Z0256193A</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>190.3</v>
+        <v>69.56</v>
       </c>
       <c r="F11" t="n">
-        <v>190.3</v>
+        <v>69.56</v>
       </c>
       <c r="G11" t="n">
-        <v>9389</v>
+        <v>3921</v>
       </c>
       <c r="H11" t="n">
-        <v>24630</v>
+        <v>15815.76</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -1799,7 +1799,7 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>190.3</v>
+        <v>69.56</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
@@ -1811,13 +1811,13 @@
         <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>24630</v>
+        <v>15815.76</v>
       </c>
       <c r="Q11" t="n">
         <v>0</v>
       </c>
       <c r="R11" t="n">
-        <v>52.86</v>
+        <v>19.32</v>
       </c>
       <c r="S11" t="n">
         <v>0</v>
@@ -1829,10 +1829,10 @@
         <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>52.86</v>
+        <v>19.32</v>
       </c>
       <c r="W11" t="n">
-        <v>52.86</v>
+        <v>19.32</v>
       </c>
       <c r="X11" t="n">
         <v>0</v>
@@ -1841,28 +1841,28 @@
         <v>0</v>
       </c>
       <c r="Z11" t="n">
-        <v>102.05</v>
+        <v>42.94</v>
       </c>
       <c r="AA11" t="n">
-        <v>24.63</v>
+        <v>15.82</v>
       </c>
       <c r="AB11" t="n">
         <v>0</v>
       </c>
       <c r="AC11" t="n">
-        <v>24.63</v>
+        <v>15.82</v>
       </c>
       <c r="AD11" t="n">
         <v>0</v>
       </c>
       <c r="AE11" t="n">
-        <v>68.22</v>
+        <v>54.99</v>
       </c>
       <c r="AF11" t="n">
         <v>0</v>
       </c>
       <c r="AG11" t="n">
-        <v>31.78</v>
+        <v>45.01</v>
       </c>
       <c r="AH11" t="inlineStr">
         <is>
@@ -1891,42 +1891,42 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Jiráskova 19/9890, Smiřice</t>
+          <t>ČEZ Energo, s.r.o., Sídliště 9890, Smiřice</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>27ZG500Z0291896F</t>
+          <t>27ZG500Z02916194</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>49.2</v>
+        <v>1148.1</v>
       </c>
       <c r="F12" t="n">
-        <v>49.2</v>
+        <v>1095.5</v>
       </c>
       <c r="G12" t="n">
-        <v>1811.01</v>
+        <v>44439</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>71321</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>52.6</v>
       </c>
       <c r="K12" t="n">
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>49.2</v>
+        <v>1095.5</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
@@ -1938,28 +1938,28 @@
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>0</v>
+        <v>71321</v>
       </c>
       <c r="Q12" t="n">
         <v>0</v>
       </c>
       <c r="R12" t="n">
-        <v>13.67</v>
+        <v>318.92</v>
       </c>
       <c r="S12" t="n">
         <v>0</v>
       </c>
       <c r="T12" t="n">
-        <v>0</v>
+        <v>14.61</v>
       </c>
       <c r="U12" t="n">
         <v>0</v>
       </c>
       <c r="V12" t="n">
-        <v>13.67</v>
+        <v>304.31</v>
       </c>
       <c r="W12" t="n">
-        <v>13.67</v>
+        <v>304.31</v>
       </c>
       <c r="X12" t="n">
         <v>0</v>
@@ -1968,39 +1968,39 @@
         <v>0</v>
       </c>
       <c r="Z12" t="n">
-        <v>19.68</v>
+        <v>483.94</v>
       </c>
       <c r="AA12" t="n">
-        <v>0</v>
+        <v>71.31999999999999</v>
       </c>
       <c r="AB12" t="n">
         <v>0</v>
       </c>
       <c r="AC12" t="n">
-        <v>0</v>
+        <v>71.31999999999999</v>
       </c>
       <c r="AD12" t="n">
         <v>0</v>
       </c>
       <c r="AE12" t="n">
-        <v>100</v>
+        <v>81.72</v>
       </c>
       <c r="AF12" t="n">
         <v>0</v>
       </c>
       <c r="AG12" t="n">
-        <v>0</v>
+        <v>18.28</v>
       </c>
       <c r="AH12" t="inlineStr">
         <is>
+          <t>ANO</t>
+        </is>
+      </c>
+      <c r="AI12" t="inlineStr">
+        <is>
           <t>NE</t>
         </is>
       </c>
-      <c r="AI12" t="inlineStr">
-        <is>
-          <t>NE</t>
-        </is>
-      </c>
       <c r="AJ12" t="inlineStr">
         <is>
           <t>ANO</t>
@@ -2008,7 +2008,7 @@
       </c>
       <c r="AK12" t="inlineStr">
         <is>
-          <t>DK</t>
+          <t>O</t>
         </is>
       </c>
     </row>
@@ -2018,27 +2018,27 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Jiráskova  206, Smiřice</t>
+          <t>ČEZ Energo, s.r.o., Jiráskova 19/9890, Smiřice</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>27ZG500Z0291801F</t>
+          <t>27ZG500Z0291896F</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>345.6</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>345.6</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>10877.78</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -2053,7 +2053,7 @@
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>345.6</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
@@ -2071,7 +2071,7 @@
         <v>0</v>
       </c>
       <c r="R13" t="n">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="S13" t="n">
         <v>0</v>
@@ -2083,10 +2083,10 @@
         <v>0</v>
       </c>
       <c r="V13" t="n">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="W13" t="n">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="X13" t="n">
         <v>0</v>
@@ -2095,7 +2095,7 @@
         <v>0</v>
       </c>
       <c r="Z13" t="n">
-        <v>0</v>
+        <v>118.46</v>
       </c>
       <c r="AA13" t="n">
         <v>0</v>
@@ -2110,7 +2110,7 @@
         <v>0</v>
       </c>
       <c r="AE13" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AF13" t="n">
         <v>0</v>
@@ -2120,7 +2120,7 @@
       </c>
       <c r="AH13" t="inlineStr">
         <is>
-          <t>ANO</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="AI13" t="inlineStr">
@@ -2135,7 +2135,7 @@
       </c>
       <c r="AK13" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>DK</t>
         </is>
       </c>
     </row>
@@ -2145,42 +2145,42 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Karla Čapka, Volyně</t>
+          <t>ČEZ Energo, s.r.o., Jiráskova  206, Smiřice</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>27ZG900Z1010705M</t>
+          <t>27ZG500Z0291801F</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>294.18</v>
+        <v>323.1</v>
       </c>
       <c r="F14" t="n">
-        <v>208.31</v>
+        <v>323.1</v>
       </c>
       <c r="G14" t="n">
-        <v>18055.89</v>
+        <v>10112.85</v>
       </c>
       <c r="H14" t="n">
-        <v>69620</v>
+        <v>5113</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>85.87</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>208.31</v>
+        <v>323.1</v>
       </c>
       <c r="M14" t="n">
         <v>0</v>
@@ -2192,28 +2192,28 @@
         <v>0</v>
       </c>
       <c r="P14" t="n">
-        <v>69620</v>
+        <v>5113</v>
       </c>
       <c r="Q14" t="n">
         <v>0</v>
       </c>
       <c r="R14" t="n">
-        <v>81.72</v>
+        <v>89.75</v>
       </c>
       <c r="S14" t="n">
         <v>0</v>
       </c>
       <c r="T14" t="n">
-        <v>23.85</v>
+        <v>0</v>
       </c>
       <c r="U14" t="n">
         <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>57.86</v>
+        <v>89.75</v>
       </c>
       <c r="W14" t="n">
-        <v>57.86</v>
+        <v>89.75</v>
       </c>
       <c r="X14" t="n">
         <v>0</v>
@@ -2222,28 +2222,28 @@
         <v>0</v>
       </c>
       <c r="Z14" t="n">
-        <v>198.02</v>
+        <v>110.13</v>
       </c>
       <c r="AA14" t="n">
-        <v>69.62</v>
+        <v>5.11</v>
       </c>
       <c r="AB14" t="n">
         <v>0</v>
       </c>
       <c r="AC14" t="n">
-        <v>69.62</v>
+        <v>5.11</v>
       </c>
       <c r="AD14" t="n">
         <v>0</v>
       </c>
       <c r="AE14" t="n">
-        <v>54</v>
+        <v>94.61</v>
       </c>
       <c r="AF14" t="n">
         <v>0</v>
       </c>
       <c r="AG14" t="n">
-        <v>46</v>
+        <v>5.39</v>
       </c>
       <c r="AH14" t="inlineStr">
         <is>
@@ -2272,42 +2272,42 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o.,Bělíkova 1398 Frýdlant</t>
+          <t>ČEZ Energo, s.r.o., Karla Čapka, Volyně</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>27ZG400Z0317866A</t>
+          <t>27ZG900Z1010705M</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>1156</v>
+        <v>1649.42</v>
       </c>
       <c r="F15" t="n">
-        <v>1156</v>
+        <v>1496.82</v>
       </c>
       <c r="G15" t="n">
-        <v>76609</v>
+        <v>80336.10000000001</v>
       </c>
       <c r="H15" t="n">
-        <v>302362</v>
+        <v>265575</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>152.6</v>
       </c>
       <c r="K15" t="n">
         <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>1156</v>
+        <v>1496.82</v>
       </c>
       <c r="M15" t="n">
         <v>0</v>
@@ -2319,28 +2319,28 @@
         <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>302362</v>
+        <v>265575</v>
       </c>
       <c r="Q15" t="n">
         <v>0</v>
       </c>
       <c r="R15" t="n">
-        <v>321.11</v>
+        <v>458.17</v>
       </c>
       <c r="S15" t="n">
         <v>0</v>
       </c>
       <c r="T15" t="n">
-        <v>0</v>
+        <v>42.39</v>
       </c>
       <c r="U15" t="n">
         <v>0</v>
       </c>
       <c r="V15" t="n">
-        <v>321.11</v>
+        <v>415.78</v>
       </c>
       <c r="W15" t="n">
-        <v>321.11</v>
+        <v>415.78</v>
       </c>
       <c r="X15" t="n">
         <v>0</v>
@@ -2349,28 +2349,28 @@
         <v>0</v>
       </c>
       <c r="Z15" t="n">
-        <v>827.03</v>
+        <v>875.66</v>
       </c>
       <c r="AA15" t="n">
-        <v>302.36</v>
+        <v>265.58</v>
       </c>
       <c r="AB15" t="n">
         <v>0</v>
       </c>
       <c r="AC15" t="n">
-        <v>302.36</v>
+        <v>265.58</v>
       </c>
       <c r="AD15" t="n">
         <v>0</v>
       </c>
       <c r="AE15" t="n">
-        <v>51.5</v>
+        <v>63.31</v>
       </c>
       <c r="AF15" t="n">
         <v>0</v>
       </c>
       <c r="AG15" t="n">
-        <v>48.5</v>
+        <v>36.69</v>
       </c>
       <c r="AH15" t="inlineStr">
         <is>
@@ -2399,30 +2399,30 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., U Břízek , Jihlava</t>
+          <t>ČEZ Energo, s.r.o.,Bělíkova 1398 Frýdlant</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>27ZG600Z06765231</t>
+          <t>27ZG400Z0317866A</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>1291</v>
+        <v>5234</v>
       </c>
       <c r="F16" t="n">
-        <v>1291</v>
+        <v>5234</v>
       </c>
       <c r="G16" t="n">
-        <v>77527</v>
+        <v>243408</v>
       </c>
       <c r="H16" t="n">
-        <v>316581</v>
+        <v>641296</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -2434,7 +2434,7 @@
         <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>1291</v>
+        <v>5234</v>
       </c>
       <c r="M16" t="n">
         <v>0</v>
@@ -2446,13 +2446,13 @@
         <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>316581</v>
+        <v>641296</v>
       </c>
       <c r="Q16" t="n">
         <v>0</v>
       </c>
       <c r="R16" t="n">
-        <v>358.61</v>
+        <v>1453.89</v>
       </c>
       <c r="S16" t="n">
         <v>0</v>
@@ -2464,10 +2464,10 @@
         <v>0</v>
       </c>
       <c r="V16" t="n">
-        <v>358.61</v>
+        <v>1453.89</v>
       </c>
       <c r="W16" t="n">
-        <v>358.61</v>
+        <v>1453.89</v>
       </c>
       <c r="X16" t="n">
         <v>0</v>
@@ -2476,28 +2476,28 @@
         <v>0</v>
       </c>
       <c r="Z16" t="n">
-        <v>836.9400000000001</v>
+        <v>2627.71</v>
       </c>
       <c r="AA16" t="n">
-        <v>316.58</v>
+        <v>641.3</v>
       </c>
       <c r="AB16" t="n">
         <v>0</v>
       </c>
       <c r="AC16" t="n">
-        <v>316.58</v>
+        <v>641.3</v>
       </c>
       <c r="AD16" t="n">
         <v>0</v>
       </c>
       <c r="AE16" t="n">
-        <v>53.11</v>
+        <v>69.39</v>
       </c>
       <c r="AF16" t="n">
         <v>0</v>
       </c>
       <c r="AG16" t="n">
-        <v>46.89</v>
+        <v>30.61</v>
       </c>
       <c r="AH16" t="inlineStr">
         <is>
@@ -2526,30 +2526,30 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Osecká  1, Duchcov</t>
+          <t>ČEZ Energo, s.r.o., U Břízek , Jihlava</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>27ZG400Z0317667G</t>
+          <t>27ZG600Z06765231</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>992.9</v>
+        <v>1573</v>
       </c>
       <c r="F17" t="n">
-        <v>992.9</v>
+        <v>1573</v>
       </c>
       <c r="G17" t="n">
-        <v>62238</v>
+        <v>92031</v>
       </c>
       <c r="H17" t="n">
-        <v>246965</v>
+        <v>379858</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -2561,7 +2561,7 @@
         <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>992.9</v>
+        <v>1573</v>
       </c>
       <c r="M17" t="n">
         <v>0</v>
@@ -2573,13 +2573,13 @@
         <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>246965</v>
+        <v>379858</v>
       </c>
       <c r="Q17" t="n">
         <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>275.81</v>
+        <v>436.94</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -2591,10 +2591,10 @@
         <v>0</v>
       </c>
       <c r="V17" t="n">
-        <v>275.81</v>
+        <v>436.94</v>
       </c>
       <c r="W17" t="n">
-        <v>275.81</v>
+        <v>436.94</v>
       </c>
       <c r="X17" t="n">
         <v>0</v>
@@ -2603,28 +2603,28 @@
         <v>0</v>
       </c>
       <c r="Z17" t="n">
-        <v>682.7</v>
+        <v>993.52</v>
       </c>
       <c r="AA17" t="n">
-        <v>246.96</v>
+        <v>379.86</v>
       </c>
       <c r="AB17" t="n">
         <v>0</v>
       </c>
       <c r="AC17" t="n">
-        <v>246.96</v>
+        <v>379.86</v>
       </c>
       <c r="AD17" t="n">
         <v>0</v>
       </c>
       <c r="AE17" t="n">
-        <v>52.76</v>
+        <v>53.49</v>
       </c>
       <c r="AF17" t="n">
         <v>0</v>
       </c>
       <c r="AG17" t="n">
-        <v>47.24</v>
+        <v>46.51</v>
       </c>
       <c r="AH17" t="inlineStr">
         <is>
@@ -2653,30 +2653,30 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Sokolská , Osek</t>
+          <t>ČEZ Energo, s.r.o., Osecká  1, Duchcov</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>27ZG400Z0318618O</t>
+          <t>27ZG400Z0317667G</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>112.2</v>
+        <v>5033.3</v>
       </c>
       <c r="F18" t="n">
-        <v>112.2</v>
+        <v>5033.3</v>
       </c>
       <c r="G18" t="n">
-        <v>6805</v>
+        <v>239051</v>
       </c>
       <c r="H18" t="n">
-        <v>23091</v>
+        <v>741823</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -2688,7 +2688,7 @@
         <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>112.2</v>
+        <v>5033.3</v>
       </c>
       <c r="M18" t="n">
         <v>0</v>
@@ -2700,13 +2700,13 @@
         <v>0</v>
       </c>
       <c r="P18" t="n">
-        <v>23091</v>
+        <v>741823</v>
       </c>
       <c r="Q18" t="n">
         <v>0</v>
       </c>
       <c r="R18" t="n">
-        <v>31.17</v>
+        <v>1398.14</v>
       </c>
       <c r="S18" t="n">
         <v>0</v>
@@ -2718,10 +2718,10 @@
         <v>0</v>
       </c>
       <c r="V18" t="n">
-        <v>31.17</v>
+        <v>1398.14</v>
       </c>
       <c r="W18" t="n">
-        <v>31.17</v>
+        <v>1398.14</v>
       </c>
       <c r="X18" t="n">
         <v>0</v>
@@ -2730,28 +2730,28 @@
         <v>0</v>
       </c>
       <c r="Z18" t="n">
-        <v>74.64</v>
+        <v>2580.68</v>
       </c>
       <c r="AA18" t="n">
-        <v>23.09</v>
+        <v>741.8200000000001</v>
       </c>
       <c r="AB18" t="n">
         <v>0</v>
       </c>
       <c r="AC18" t="n">
-        <v>23.09</v>
+        <v>741.8200000000001</v>
       </c>
       <c r="AD18" t="n">
         <v>0</v>
       </c>
       <c r="AE18" t="n">
-        <v>57.44</v>
+        <v>65.33</v>
       </c>
       <c r="AF18" t="n">
         <v>0</v>
       </c>
       <c r="AG18" t="n">
-        <v>42.56</v>
+        <v>34.67</v>
       </c>
       <c r="AH18" t="inlineStr">
         <is>
@@ -2780,30 +2780,30 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Hornická 746, Bystřice nad Perštejnem</t>
+          <t>ČEZ Energo, s.r.o., Sokolská , Osek</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>27ZG600Z0695755A</t>
+          <t>27ZG400Z0318618O</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>580.5</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>580.5</v>
       </c>
       <c r="G19" t="n">
-        <v>84</v>
+        <v>25210</v>
       </c>
       <c r="H19" t="n">
-        <v>295</v>
+        <v>61462</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
@@ -2815,7 +2815,7 @@
         <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>580.5</v>
       </c>
       <c r="M19" t="n">
         <v>0</v>
@@ -2827,13 +2827,13 @@
         <v>0</v>
       </c>
       <c r="P19" t="n">
-        <v>295</v>
+        <v>61462</v>
       </c>
       <c r="Q19" t="n">
         <v>0</v>
       </c>
       <c r="R19" t="n">
-        <v>0</v>
+        <v>161.25</v>
       </c>
       <c r="S19" t="n">
         <v>0</v>
@@ -2845,10 +2845,10 @@
         <v>0</v>
       </c>
       <c r="V19" t="n">
-        <v>0</v>
+        <v>161.25</v>
       </c>
       <c r="W19" t="n">
-        <v>0</v>
+        <v>161.25</v>
       </c>
       <c r="X19" t="n">
         <v>0</v>
@@ -2857,28 +2857,28 @@
         <v>0</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.91</v>
+        <v>274.79</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.3</v>
+        <v>61.46</v>
       </c>
       <c r="AB19" t="n">
         <v>0</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.3</v>
+        <v>61.46</v>
       </c>
       <c r="AD19" t="n">
         <v>0</v>
       </c>
       <c r="AE19" t="n">
-        <v>0</v>
+        <v>72.40000000000001</v>
       </c>
       <c r="AF19" t="n">
         <v>0</v>
       </c>
       <c r="AG19" t="n">
-        <v>0</v>
+        <v>27.6</v>
       </c>
       <c r="AH19" t="inlineStr">
         <is>
@@ -2907,30 +2907,30 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ČEZ Energo,s .r.o., Malé nám. 830 Votice</t>
+          <t>ČEZ Energo, s.r.o., Hornická 746, Bystřice nad Perštejnem</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>27ZG200Z0235914H</t>
+          <t>27ZG600Z0695755A</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>530</v>
+        <v>3693.65</v>
       </c>
       <c r="F20" t="n">
-        <v>530</v>
+        <v>3693.65</v>
       </c>
       <c r="G20" t="n">
-        <v>27117</v>
+        <v>227790</v>
       </c>
       <c r="H20" t="n">
-        <v>77791</v>
+        <v>933000</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
@@ -2942,7 +2942,7 @@
         <v>0</v>
       </c>
       <c r="L20" t="n">
-        <v>530</v>
+        <v>3693.65</v>
       </c>
       <c r="M20" t="n">
         <v>0</v>
@@ -2954,13 +2954,13 @@
         <v>0</v>
       </c>
       <c r="P20" t="n">
-        <v>77791</v>
+        <v>933000</v>
       </c>
       <c r="Q20" t="n">
         <v>0</v>
       </c>
       <c r="R20" t="n">
-        <v>147.22</v>
+        <v>1026.02</v>
       </c>
       <c r="S20" t="n">
         <v>0</v>
@@ -2972,10 +2972,10 @@
         <v>0</v>
       </c>
       <c r="V20" t="n">
-        <v>147.22</v>
+        <v>1026.02</v>
       </c>
       <c r="W20" t="n">
-        <v>147.22</v>
+        <v>1026.02</v>
       </c>
       <c r="X20" t="n">
         <v>0</v>
@@ -2984,28 +2984,28 @@
         <v>0</v>
       </c>
       <c r="Z20" t="n">
-        <v>297.78</v>
+        <v>2459.11</v>
       </c>
       <c r="AA20" t="n">
-        <v>77.79000000000001</v>
+        <v>933</v>
       </c>
       <c r="AB20" t="n">
         <v>0</v>
       </c>
       <c r="AC20" t="n">
-        <v>77.79000000000001</v>
+        <v>933</v>
       </c>
       <c r="AD20" t="n">
         <v>0</v>
       </c>
       <c r="AE20" t="n">
-        <v>65.43000000000001</v>
+        <v>52.37</v>
       </c>
       <c r="AF20" t="n">
         <v>0</v>
       </c>
       <c r="AG20" t="n">
-        <v>34.57</v>
+        <v>47.63</v>
       </c>
       <c r="AH20" t="inlineStr">
         <is>
@@ -3034,30 +3034,30 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Fügnerova 572, Vrchlabí (AZ)</t>
+          <t>ČEZ Energo,s .r.o., Malé nám. 830 Votice</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>27ZG500Z03218136</t>
+          <t>27ZG200Z0235914H</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>432</v>
+        <v>2493.09</v>
       </c>
       <c r="F21" t="n">
-        <v>432</v>
+        <v>2493.09</v>
       </c>
       <c r="G21" t="n">
-        <v>25657</v>
+        <v>122606.2</v>
       </c>
       <c r="H21" t="n">
-        <v>102014</v>
+        <v>343380.67</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
@@ -3069,7 +3069,7 @@
         <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>432</v>
+        <v>2493.09</v>
       </c>
       <c r="M21" t="n">
         <v>0</v>
@@ -3081,13 +3081,13 @@
         <v>0</v>
       </c>
       <c r="P21" t="n">
-        <v>102014</v>
+        <v>343380.67</v>
       </c>
       <c r="Q21" t="n">
         <v>0</v>
       </c>
       <c r="R21" t="n">
-        <v>120</v>
+        <v>692.53</v>
       </c>
       <c r="S21" t="n">
         <v>0</v>
@@ -3099,10 +3099,10 @@
         <v>0</v>
       </c>
       <c r="V21" t="n">
-        <v>120</v>
+        <v>692.53</v>
       </c>
       <c r="W21" t="n">
-        <v>120</v>
+        <v>692.53</v>
       </c>
       <c r="X21" t="n">
         <v>0</v>
@@ -3111,28 +3111,28 @@
         <v>0</v>
       </c>
       <c r="Z21" t="n">
-        <v>281.59</v>
+        <v>1338.36</v>
       </c>
       <c r="AA21" t="n">
-        <v>102.01</v>
+        <v>343.38</v>
       </c>
       <c r="AB21" t="n">
         <v>0</v>
       </c>
       <c r="AC21" t="n">
-        <v>102.01</v>
+        <v>343.38</v>
       </c>
       <c r="AD21" t="n">
         <v>0</v>
       </c>
       <c r="AE21" t="n">
-        <v>54.05</v>
+        <v>66.84999999999999</v>
       </c>
       <c r="AF21" t="n">
         <v>0</v>
       </c>
       <c r="AG21" t="n">
-        <v>45.95</v>
+        <v>33.15</v>
       </c>
       <c r="AH21" t="inlineStr">
         <is>
@@ -3161,30 +3161,30 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Českých  bratří 509, Vrchlabí (NKTC)</t>
+          <t>ČEZ Energo, s.r.o., Fügnerova 572, Vrchlabí (AZ)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>27ZG500Z02917077</t>
+          <t>27ZG500Z03218136</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>1502</v>
+        <v>182</v>
       </c>
       <c r="F22" t="n">
-        <v>1502</v>
+        <v>182</v>
       </c>
       <c r="G22" t="n">
-        <v>88235</v>
+        <v>11122</v>
       </c>
       <c r="H22" t="n">
-        <v>360972</v>
+        <v>42783</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
@@ -3196,7 +3196,7 @@
         <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>1502</v>
+        <v>182</v>
       </c>
       <c r="M22" t="n">
         <v>0</v>
@@ -3208,13 +3208,13 @@
         <v>0</v>
       </c>
       <c r="P22" t="n">
-        <v>360972</v>
+        <v>42783</v>
       </c>
       <c r="Q22" t="n">
         <v>0</v>
       </c>
       <c r="R22" t="n">
-        <v>417.22</v>
+        <v>50.56</v>
       </c>
       <c r="S22" t="n">
         <v>0</v>
@@ -3226,10 +3226,10 @@
         <v>0</v>
       </c>
       <c r="V22" t="n">
-        <v>417.22</v>
+        <v>50.56</v>
       </c>
       <c r="W22" t="n">
-        <v>417.22</v>
+        <v>50.56</v>
       </c>
       <c r="X22" t="n">
         <v>0</v>
@@ -3238,28 +3238,28 @@
         <v>0</v>
       </c>
       <c r="Z22" t="n">
-        <v>968.41</v>
+        <v>121.23</v>
       </c>
       <c r="AA22" t="n">
-        <v>360.97</v>
+        <v>42.78</v>
       </c>
       <c r="AB22" t="n">
         <v>0</v>
       </c>
       <c r="AC22" t="n">
-        <v>360.97</v>
+        <v>42.78</v>
       </c>
       <c r="AD22" t="n">
         <v>0</v>
       </c>
       <c r="AE22" t="n">
-        <v>53.61</v>
+        <v>54.16</v>
       </c>
       <c r="AF22" t="n">
         <v>0</v>
       </c>
       <c r="AG22" t="n">
-        <v>46.39</v>
+        <v>45.84</v>
       </c>
       <c r="AH22" t="inlineStr">
         <is>
@@ -3288,30 +3288,30 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Dukelských hrdinů 28, Krupka</t>
+          <t>ČEZ Energo, s.r.o., Českých  bratří 509, Vrchlabí (NKTC)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>27ZG400Z0318329V</t>
+          <t>27ZG500Z02917077</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>770.96</v>
+        <v>5674.99</v>
       </c>
       <c r="F23" t="n">
-        <v>770.96</v>
+        <v>5674.99</v>
       </c>
       <c r="G23" t="n">
-        <v>33095</v>
+        <v>327256</v>
       </c>
       <c r="H23" t="n">
-        <v>98975</v>
+        <v>1328970</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
@@ -3323,7 +3323,7 @@
         <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>770.96</v>
+        <v>5674.99</v>
       </c>
       <c r="M23" t="n">
         <v>0</v>
@@ -3335,13 +3335,13 @@
         <v>0</v>
       </c>
       <c r="P23" t="n">
-        <v>98975</v>
+        <v>1328970</v>
       </c>
       <c r="Q23" t="n">
         <v>0</v>
       </c>
       <c r="R23" t="n">
-        <v>214.16</v>
+        <v>1576.39</v>
       </c>
       <c r="S23" t="n">
         <v>0</v>
@@ -3353,10 +3353,10 @@
         <v>0</v>
       </c>
       <c r="V23" t="n">
-        <v>214.16</v>
+        <v>1576.39</v>
       </c>
       <c r="W23" t="n">
-        <v>214.16</v>
+        <v>1576.39</v>
       </c>
       <c r="X23" t="n">
         <v>0</v>
@@ -3365,28 +3365,28 @@
         <v>0</v>
       </c>
       <c r="Z23" t="n">
-        <v>363.03</v>
+        <v>3567.09</v>
       </c>
       <c r="AA23" t="n">
-        <v>98.98</v>
+        <v>1328.97</v>
       </c>
       <c r="AB23" t="n">
         <v>0</v>
       </c>
       <c r="AC23" t="n">
-        <v>98.98</v>
+        <v>1328.97</v>
       </c>
       <c r="AD23" t="n">
         <v>0</v>
       </c>
       <c r="AE23" t="n">
-        <v>68.39</v>
+        <v>54.26</v>
       </c>
       <c r="AF23" t="n">
         <v>0</v>
       </c>
       <c r="AG23" t="n">
-        <v>31.61</v>
+        <v>45.74</v>
       </c>
       <c r="AH23" t="inlineStr">
         <is>
@@ -3415,30 +3415,30 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Dukelská , Vrchlabí</t>
+          <t>ČEZ Energo, s.r.o., Dukelských hrdinů 28, Krupka</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>27ZG500Z0292130V</t>
+          <t>27ZG400Z0318329V</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>24.72</v>
+        <v>3804.21</v>
       </c>
       <c r="F24" t="n">
-        <v>24.72</v>
+        <v>3804.21</v>
       </c>
       <c r="G24" t="n">
-        <v>680</v>
+        <v>161122</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>482299</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
@@ -3450,7 +3450,7 @@
         <v>0</v>
       </c>
       <c r="L24" t="n">
-        <v>24.72</v>
+        <v>3804.21</v>
       </c>
       <c r="M24" t="n">
         <v>0</v>
@@ -3462,13 +3462,13 @@
         <v>0</v>
       </c>
       <c r="P24" t="n">
-        <v>0</v>
+        <v>482299</v>
       </c>
       <c r="Q24" t="n">
         <v>0</v>
       </c>
       <c r="R24" t="n">
-        <v>6.87</v>
+        <v>1056.73</v>
       </c>
       <c r="S24" t="n">
         <v>0</v>
@@ -3480,10 +3480,10 @@
         <v>0</v>
       </c>
       <c r="V24" t="n">
-        <v>6.87</v>
+        <v>1056.73</v>
       </c>
       <c r="W24" t="n">
-        <v>6.87</v>
+        <v>1056.73</v>
       </c>
       <c r="X24" t="n">
         <v>0</v>
@@ -3492,32 +3492,32 @@
         <v>0</v>
       </c>
       <c r="Z24" t="n">
-        <v>7.46</v>
+        <v>1739.39</v>
       </c>
       <c r="AA24" t="n">
-        <v>0</v>
+        <v>482.3</v>
       </c>
       <c r="AB24" t="n">
         <v>0</v>
       </c>
       <c r="AC24" t="n">
-        <v>0</v>
+        <v>482.3</v>
       </c>
       <c r="AD24" t="n">
         <v>0</v>
       </c>
       <c r="AE24" t="n">
-        <v>100</v>
+        <v>68.66</v>
       </c>
       <c r="AF24" t="n">
         <v>0</v>
       </c>
       <c r="AG24" t="n">
-        <v>0</v>
+        <v>31.34</v>
       </c>
       <c r="AH24" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t>ANO</t>
         </is>
       </c>
       <c r="AI24" t="inlineStr">
@@ -3542,30 +3542,30 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Bojkovice</t>
+          <t>ČEZ Energo, s.r.o., Dukelská , Vrchlabí</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>27ZG600Z0002166T</t>
+          <t>27ZG500Z0292130V</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>24</v>
+        <v>6548.04</v>
       </c>
       <c r="F25" t="n">
-        <v>24</v>
+        <v>6548.04</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>181382</v>
       </c>
       <c r="H25" t="n">
-        <v>147367159</v>
+        <v>0</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
@@ -3577,10 +3577,10 @@
         <v>0</v>
       </c>
       <c r="L25" t="n">
-        <v>0</v>
+        <v>6548.04</v>
       </c>
       <c r="M25" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N25" t="n">
         <v>0</v>
@@ -3589,13 +3589,13 @@
         <v>0</v>
       </c>
       <c r="P25" t="n">
-        <v>147367159</v>
+        <v>0</v>
       </c>
       <c r="Q25" t="n">
         <v>0</v>
       </c>
       <c r="R25" t="n">
-        <v>6.67</v>
+        <v>1818.9</v>
       </c>
       <c r="S25" t="n">
         <v>0</v>
@@ -3607,34 +3607,34 @@
         <v>0</v>
       </c>
       <c r="V25" t="n">
-        <v>6.67</v>
+        <v>1818.9</v>
       </c>
       <c r="W25" t="n">
-        <v>0</v>
+        <v>1818.9</v>
       </c>
       <c r="X25" t="n">
-        <v>6.67</v>
+        <v>0</v>
       </c>
       <c r="Y25" t="n">
         <v>0</v>
       </c>
       <c r="Z25" t="n">
-        <v>0</v>
+        <v>1977.06</v>
       </c>
       <c r="AA25" t="n">
-        <v>147367.16</v>
+        <v>0</v>
       </c>
       <c r="AB25" t="n">
         <v>0</v>
       </c>
       <c r="AC25" t="n">
-        <v>147367.16</v>
+        <v>0</v>
       </c>
       <c r="AD25" t="n">
         <v>0</v>
       </c>
       <c r="AE25" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AF25" t="n">
         <v>0</v>
@@ -3644,7 +3644,7 @@
       </c>
       <c r="AH25" t="inlineStr">
         <is>
-          <t>ANO</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="AI25" t="inlineStr">
@@ -3654,12 +3654,12 @@
       </c>
       <c r="AJ25" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t>ANO</t>
         </is>
       </c>
       <c r="AK25" t="inlineStr">
         <is>
-          <t>Z1</t>
+          <t>O</t>
         </is>
       </c>
     </row>
@@ -3669,30 +3669,30 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Kladruby 30</t>
+          <t>ČEZ Energo, s.r.o., Bojkovice</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>27ZG200Z0235827C</t>
+          <t>27ZG600Z0002166T</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>430.52</v>
+        <v>1798</v>
       </c>
       <c r="F26" t="n">
-        <v>430.52</v>
+        <v>1798</v>
       </c>
       <c r="G26" t="n">
-        <v>23730</v>
+        <v>107654</v>
       </c>
       <c r="H26" t="n">
-        <v>82261</v>
+        <v>436410</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
@@ -3707,7 +3707,7 @@
         <v>0</v>
       </c>
       <c r="M26" t="n">
-        <v>430.52</v>
+        <v>1798</v>
       </c>
       <c r="N26" t="n">
         <v>0</v>
@@ -3716,13 +3716,13 @@
         <v>0</v>
       </c>
       <c r="P26" t="n">
-        <v>82261</v>
+        <v>436410</v>
       </c>
       <c r="Q26" t="n">
         <v>0</v>
       </c>
       <c r="R26" t="n">
-        <v>119.59</v>
+        <v>499.44</v>
       </c>
       <c r="S26" t="n">
         <v>0</v>
@@ -3734,28 +3734,28 @@
         <v>0</v>
       </c>
       <c r="V26" t="n">
-        <v>119.59</v>
+        <v>499.44</v>
       </c>
       <c r="W26" t="n">
         <v>0</v>
       </c>
       <c r="X26" t="n">
-        <v>119.59</v>
+        <v>499.44</v>
       </c>
       <c r="Y26" t="n">
         <v>0</v>
       </c>
       <c r="Z26" t="n">
-        <v>260.6</v>
+        <v>1162.18</v>
       </c>
       <c r="AA26" t="n">
-        <v>82.26000000000001</v>
+        <v>436.41</v>
       </c>
       <c r="AB26" t="n">
         <v>0</v>
       </c>
       <c r="AC26" t="n">
-        <v>82.26000000000001</v>
+        <v>436.41</v>
       </c>
       <c r="AD26" t="n">
         <v>0</v>
@@ -3764,10 +3764,10 @@
         <v>0</v>
       </c>
       <c r="AF26" t="n">
-        <v>59.25</v>
+        <v>53.37</v>
       </c>
       <c r="AG26" t="n">
-        <v>40.75</v>
+        <v>46.63</v>
       </c>
       <c r="AH26" t="inlineStr">
         <is>
@@ -3796,30 +3796,30 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Zahradní 313, 373 33 Nové Hrady</t>
+          <t>ČEZ Energo, s.r.o., Kladruby 30</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>27ZG900Z10114758</t>
+          <t>27ZG200Z0235827C</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>1655.78</v>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
+        <v>1655.78</v>
       </c>
       <c r="G27" t="n">
-        <v>5703</v>
+        <v>88831</v>
       </c>
       <c r="H27" t="n">
-        <v>14340</v>
+        <v>316761</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
@@ -3834,7 +3834,7 @@
         <v>0</v>
       </c>
       <c r="M27" t="n">
-        <v>0</v>
+        <v>1655.78</v>
       </c>
       <c r="N27" t="n">
         <v>0</v>
@@ -3843,13 +3843,13 @@
         <v>0</v>
       </c>
       <c r="P27" t="n">
-        <v>14340</v>
+        <v>316761</v>
       </c>
       <c r="Q27" t="n">
         <v>0</v>
       </c>
       <c r="R27" t="n">
-        <v>0</v>
+        <v>459.94</v>
       </c>
       <c r="S27" t="n">
         <v>0</v>
@@ -3861,28 +3861,28 @@
         <v>0</v>
       </c>
       <c r="V27" t="n">
-        <v>0</v>
+        <v>459.94</v>
       </c>
       <c r="W27" t="n">
         <v>0</v>
       </c>
       <c r="X27" t="n">
-        <v>0</v>
+        <v>459.94</v>
       </c>
       <c r="Y27" t="n">
         <v>0</v>
       </c>
       <c r="Z27" t="n">
-        <v>62.54</v>
+        <v>968.26</v>
       </c>
       <c r="AA27" t="n">
-        <v>14.34</v>
+        <v>316.76</v>
       </c>
       <c r="AB27" t="n">
         <v>0</v>
       </c>
       <c r="AC27" t="n">
-        <v>14.34</v>
+        <v>316.76</v>
       </c>
       <c r="AD27" t="n">
         <v>0</v>
@@ -3891,10 +3891,10 @@
         <v>0</v>
       </c>
       <c r="AF27" t="n">
-        <v>0</v>
+        <v>59.22</v>
       </c>
       <c r="AG27" t="n">
-        <v>0</v>
+        <v>40.78</v>
       </c>
       <c r="AH27" t="inlineStr">
         <is>
@@ -3908,12 +3908,12 @@
       </c>
       <c r="AJ27" t="inlineStr">
         <is>
-          <t>ANO</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="AK27" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Z1</t>
         </is>
       </c>
     </row>
@@ -3923,30 +3923,30 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Přelouč, K2 Tyršova 1004</t>
+          <t>ČEZ Energo, s.r.o., Zahradní 313, 373 33 Nové Hrady</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>27ZG500Z02918154</t>
+          <t>27ZG900Z10114758</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>41.88</v>
+        <v>459.96</v>
       </c>
       <c r="F28" t="n">
-        <v>41.88</v>
+        <v>459.96</v>
       </c>
       <c r="G28" t="n">
-        <v>1563.32</v>
+        <v>21528</v>
       </c>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>37749</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
@@ -3958,7 +3958,7 @@
         <v>0</v>
       </c>
       <c r="L28" t="n">
-        <v>41.88</v>
+        <v>459.96</v>
       </c>
       <c r="M28" t="n">
         <v>0</v>
@@ -3970,13 +3970,13 @@
         <v>0</v>
       </c>
       <c r="P28" t="n">
-        <v>0</v>
+        <v>37749</v>
       </c>
       <c r="Q28" t="n">
         <v>0</v>
       </c>
       <c r="R28" t="n">
-        <v>11.63</v>
+        <v>127.77</v>
       </c>
       <c r="S28" t="n">
         <v>0</v>
@@ -3988,10 +3988,10 @@
         <v>0</v>
       </c>
       <c r="V28" t="n">
-        <v>11.63</v>
+        <v>127.77</v>
       </c>
       <c r="W28" t="n">
-        <v>11.63</v>
+        <v>127.77</v>
       </c>
       <c r="X28" t="n">
         <v>0</v>
@@ -4000,39 +4000,39 @@
         <v>0</v>
       </c>
       <c r="Z28" t="n">
-        <v>17.16</v>
+        <v>234.84</v>
       </c>
       <c r="AA28" t="n">
-        <v>0</v>
+        <v>37.75</v>
       </c>
       <c r="AB28" t="n">
         <v>0</v>
       </c>
       <c r="AC28" t="n">
-        <v>0</v>
+        <v>37.75</v>
       </c>
       <c r="AD28" t="n">
         <v>0</v>
       </c>
       <c r="AE28" t="n">
-        <v>100</v>
+        <v>77.19</v>
       </c>
       <c r="AF28" t="n">
         <v>0</v>
       </c>
       <c r="AG28" t="n">
-        <v>0</v>
+        <v>22.81</v>
       </c>
       <c r="AH28" t="inlineStr">
         <is>
+          <t>ANO</t>
+        </is>
+      </c>
+      <c r="AI28" t="inlineStr">
+        <is>
           <t>NE</t>
         </is>
       </c>
-      <c r="AI28" t="inlineStr">
-        <is>
-          <t>NE</t>
-        </is>
-      </c>
       <c r="AJ28" t="inlineStr">
         <is>
           <t>ANO</t>
@@ -4040,7 +4040,7 @@
       </c>
       <c r="AK28" t="inlineStr">
         <is>
-          <t>DK</t>
+          <t>O</t>
         </is>
       </c>
     </row>
@@ -4050,42 +4050,42 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Přelouč, K10 nám. 17. listopadu 1518</t>
+          <t>ČEZ Energo, s.r.o., Přelouč, K2 Tyršova 1004</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>27ZG500Z0291889C</t>
+          <t>27ZG500Z02918154</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>223.1</v>
+        <v>362.3</v>
       </c>
       <c r="F29" t="n">
-        <v>150.58</v>
+        <v>339.19</v>
       </c>
       <c r="G29" t="n">
-        <v>11047</v>
+        <v>10862.46</v>
       </c>
       <c r="H29" t="n">
-        <v>33127</v>
+        <v>0</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>72.52</v>
+        <v>23.11</v>
       </c>
       <c r="K29" t="n">
         <v>0</v>
       </c>
       <c r="L29" t="n">
-        <v>150.58</v>
+        <v>339.19</v>
       </c>
       <c r="M29" t="n">
         <v>0</v>
@@ -4097,28 +4097,28 @@
         <v>0</v>
       </c>
       <c r="P29" t="n">
-        <v>33127</v>
+        <v>0</v>
       </c>
       <c r="Q29" t="n">
         <v>0</v>
       </c>
       <c r="R29" t="n">
-        <v>61.97</v>
+        <v>100.64</v>
       </c>
       <c r="S29" t="n">
         <v>0</v>
       </c>
       <c r="T29" t="n">
-        <v>20.14</v>
+        <v>6.42</v>
       </c>
       <c r="U29" t="n">
         <v>0</v>
       </c>
       <c r="V29" t="n">
-        <v>41.83</v>
+        <v>94.22</v>
       </c>
       <c r="W29" t="n">
-        <v>41.83</v>
+        <v>94.22</v>
       </c>
       <c r="X29" t="n">
         <v>0</v>
@@ -4127,32 +4127,32 @@
         <v>0</v>
       </c>
       <c r="Z29" t="n">
-        <v>121.24</v>
+        <v>118.4</v>
       </c>
       <c r="AA29" t="n">
-        <v>33.13</v>
+        <v>0</v>
       </c>
       <c r="AB29" t="n">
         <v>0</v>
       </c>
       <c r="AC29" t="n">
-        <v>33.13</v>
+        <v>0</v>
       </c>
       <c r="AD29" t="n">
         <v>0</v>
       </c>
       <c r="AE29" t="n">
-        <v>65.17</v>
+        <v>100</v>
       </c>
       <c r="AF29" t="n">
         <v>0</v>
       </c>
       <c r="AG29" t="n">
-        <v>34.83</v>
+        <v>0</v>
       </c>
       <c r="AH29" t="inlineStr">
         <is>
-          <t>ANO</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="AI29" t="inlineStr">
@@ -4167,7 +4167,7 @@
       </c>
       <c r="AK29" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>DK</t>
         </is>
       </c>
     </row>
@@ -4177,45 +4177,45 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Hrabyně, Rehab.ústav</t>
+          <t>ČEZ Energo, s.r.o., Přelouč, K10 nám. 17. listopadu 1518</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>27ZG700Z0631588A</t>
+          <t>27ZG500Z0291889C</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>568</v>
+        <v>1092.5</v>
       </c>
       <c r="F30" t="n">
-        <v>568</v>
+        <v>995.7</v>
       </c>
       <c r="G30" t="n">
-        <v>39880</v>
+        <v>43441</v>
       </c>
       <c r="H30" t="n">
-        <v>158990</v>
+        <v>87019</v>
       </c>
       <c r="I30" t="n">
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>96.8</v>
       </c>
       <c r="K30" t="n">
         <v>0</v>
       </c>
       <c r="L30" t="n">
-        <v>0</v>
+        <v>995.7</v>
       </c>
       <c r="M30" t="n">
-        <v>568</v>
+        <v>0</v>
       </c>
       <c r="N30" t="n">
         <v>0</v>
@@ -4224,58 +4224,58 @@
         <v>0</v>
       </c>
       <c r="P30" t="n">
-        <v>158990</v>
+        <v>87019</v>
       </c>
       <c r="Q30" t="n">
         <v>0</v>
       </c>
       <c r="R30" t="n">
-        <v>157.78</v>
+        <v>303.47</v>
       </c>
       <c r="S30" t="n">
         <v>0</v>
       </c>
       <c r="T30" t="n">
-        <v>0</v>
+        <v>26.89</v>
       </c>
       <c r="U30" t="n">
         <v>0</v>
       </c>
       <c r="V30" t="n">
-        <v>157.78</v>
+        <v>276.58</v>
       </c>
       <c r="W30" t="n">
-        <v>0</v>
+        <v>276.58</v>
       </c>
       <c r="X30" t="n">
-        <v>157.78</v>
+        <v>0</v>
       </c>
       <c r="Y30" t="n">
         <v>0</v>
       </c>
       <c r="Z30" t="n">
-        <v>437.45</v>
+        <v>473.51</v>
       </c>
       <c r="AA30" t="n">
-        <v>158.99</v>
+        <v>87.02</v>
       </c>
       <c r="AB30" t="n">
         <v>0</v>
       </c>
       <c r="AC30" t="n">
-        <v>158.99</v>
+        <v>87.02</v>
       </c>
       <c r="AD30" t="n">
         <v>0</v>
       </c>
       <c r="AE30" t="n">
-        <v>0</v>
+        <v>77.72</v>
       </c>
       <c r="AF30" t="n">
-        <v>49.81</v>
+        <v>0</v>
       </c>
       <c r="AG30" t="n">
-        <v>50.19</v>
+        <v>22.28</v>
       </c>
       <c r="AH30" t="inlineStr">
         <is>
@@ -4289,12 +4289,12 @@
       </c>
       <c r="AJ30" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t>ANO</t>
         </is>
       </c>
       <c r="AK30" t="inlineStr">
         <is>
-          <t>Z1</t>
+          <t>O</t>
         </is>
       </c>
     </row>
@@ -4304,45 +4304,45 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Mjr. Nováka 1477/13, Ivančice</t>
+          <t>ČEZ Energo, s.r.o., Hrabyně, Rehab.ústav</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>27ZG600Z0001733P</t>
+          <t>27ZG700Z0631588A</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1216</v>
+        <v>2157</v>
       </c>
       <c r="F31" t="n">
-        <v>843.48</v>
+        <v>2157</v>
       </c>
       <c r="G31" t="n">
-        <v>54042</v>
+        <v>136537</v>
       </c>
       <c r="H31" t="n">
-        <v>215090</v>
+        <v>543310</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>372.52</v>
+        <v>0</v>
       </c>
       <c r="K31" t="n">
         <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>843.48</v>
+        <v>0</v>
       </c>
       <c r="M31" t="n">
-        <v>0</v>
+        <v>2157</v>
       </c>
       <c r="N31" t="n">
         <v>0</v>
@@ -4351,58 +4351,58 @@
         <v>0</v>
       </c>
       <c r="P31" t="n">
-        <v>215090</v>
+        <v>543310</v>
       </c>
       <c r="Q31" t="n">
         <v>0</v>
       </c>
       <c r="R31" t="n">
-        <v>337.78</v>
+        <v>599.17</v>
       </c>
       <c r="S31" t="n">
         <v>0</v>
       </c>
       <c r="T31" t="n">
-        <v>103.48</v>
+        <v>0</v>
       </c>
       <c r="U31" t="n">
         <v>0</v>
       </c>
       <c r="V31" t="n">
-        <v>234.3</v>
+        <v>599.17</v>
       </c>
       <c r="W31" t="n">
-        <v>234.3</v>
+        <v>0</v>
       </c>
       <c r="X31" t="n">
-        <v>0</v>
+        <v>599.17</v>
       </c>
       <c r="Y31" t="n">
         <v>0</v>
       </c>
       <c r="Z31" t="n">
-        <v>592.8</v>
+        <v>1488.25</v>
       </c>
       <c r="AA31" t="n">
-        <v>215.09</v>
+        <v>543.3099999999999</v>
       </c>
       <c r="AB31" t="n">
         <v>0</v>
       </c>
       <c r="AC31" t="n">
-        <v>215.09</v>
+        <v>543.3099999999999</v>
       </c>
       <c r="AD31" t="n">
         <v>0</v>
       </c>
       <c r="AE31" t="n">
-        <v>61.1</v>
+        <v>0</v>
       </c>
       <c r="AF31" t="n">
-        <v>0</v>
+        <v>52.44</v>
       </c>
       <c r="AG31" t="n">
-        <v>38.9</v>
+        <v>47.56</v>
       </c>
       <c r="AH31" t="inlineStr">
         <is>
@@ -4416,12 +4416,12 @@
       </c>
       <c r="AJ31" t="inlineStr">
         <is>
-          <t>ANO</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="AK31" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Z1</t>
         </is>
       </c>
     </row>
@@ -4431,42 +4431,42 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., ul Nádražní Kdyně</t>
+          <t>ČEZ Energo, s.r.o., Mjr. Nováka 1477/13, Ivančice</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>27ZG302Z0000010C</t>
+          <t>27ZG600Z0001733P</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>381</v>
+        <v>5773</v>
       </c>
       <c r="F32" t="n">
-        <v>381</v>
+        <v>5179</v>
       </c>
       <c r="G32" t="n">
-        <v>23736</v>
+        <v>247204</v>
       </c>
       <c r="H32" t="n">
-        <v>94040</v>
+        <v>632430</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>0</v>
+        <v>594</v>
       </c>
       <c r="K32" t="n">
         <v>0</v>
       </c>
       <c r="L32" t="n">
-        <v>381</v>
+        <v>5179</v>
       </c>
       <c r="M32" t="n">
         <v>0</v>
@@ -4478,28 +4478,28 @@
         <v>0</v>
       </c>
       <c r="P32" t="n">
-        <v>94040</v>
+        <v>632430</v>
       </c>
       <c r="Q32" t="n">
         <v>0</v>
       </c>
       <c r="R32" t="n">
-        <v>105.83</v>
+        <v>1603.61</v>
       </c>
       <c r="S32" t="n">
         <v>0</v>
       </c>
       <c r="T32" t="n">
-        <v>0</v>
+        <v>165</v>
       </c>
       <c r="U32" t="n">
         <v>0</v>
       </c>
       <c r="V32" t="n">
-        <v>105.83</v>
+        <v>1438.61</v>
       </c>
       <c r="W32" t="n">
-        <v>105.83</v>
+        <v>1438.61</v>
       </c>
       <c r="X32" t="n">
         <v>0</v>
@@ -4508,28 +4508,28 @@
         <v>0</v>
       </c>
       <c r="Z32" t="n">
-        <v>259.58</v>
+        <v>2668.69</v>
       </c>
       <c r="AA32" t="n">
-        <v>94.04000000000001</v>
+        <v>632.4299999999999</v>
       </c>
       <c r="AB32" t="n">
         <v>0</v>
       </c>
       <c r="AC32" t="n">
-        <v>94.04000000000001</v>
+        <v>632.4299999999999</v>
       </c>
       <c r="AD32" t="n">
         <v>0</v>
       </c>
       <c r="AE32" t="n">
-        <v>52.95</v>
+        <v>71.72</v>
       </c>
       <c r="AF32" t="n">
         <v>0</v>
       </c>
       <c r="AG32" t="n">
-        <v>47.05</v>
+        <v>28.28</v>
       </c>
       <c r="AH32" t="inlineStr">
         <is>
@@ -4558,30 +4558,30 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Kotelská 9027, 337 01 Rokycany</t>
+          <t>ČEZ Energo, s.r.o., ul Nádražní Kdyně</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>27ZG300Z0249752G</t>
+          <t>27ZG302Z0000010C</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>589</v>
+        <v>1137</v>
       </c>
       <c r="F33" t="n">
-        <v>589</v>
+        <v>1137</v>
       </c>
       <c r="G33" t="n">
-        <v>29443</v>
+        <v>70549</v>
       </c>
       <c r="H33" t="n">
-        <v>101793</v>
+        <v>279250</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
@@ -4593,7 +4593,7 @@
         <v>0</v>
       </c>
       <c r="L33" t="n">
-        <v>589</v>
+        <v>1137</v>
       </c>
       <c r="M33" t="n">
         <v>0</v>
@@ -4605,13 +4605,13 @@
         <v>0</v>
       </c>
       <c r="P33" t="n">
-        <v>101793</v>
+        <v>279250</v>
       </c>
       <c r="Q33" t="n">
         <v>0</v>
       </c>
       <c r="R33" t="n">
-        <v>163.61</v>
+        <v>315.83</v>
       </c>
       <c r="S33" t="n">
         <v>0</v>
@@ -4623,10 +4623,10 @@
         <v>0</v>
       </c>
       <c r="V33" t="n">
-        <v>163.61</v>
+        <v>315.83</v>
       </c>
       <c r="W33" t="n">
-        <v>163.61</v>
+        <v>315.83</v>
       </c>
       <c r="X33" t="n">
         <v>0</v>
@@ -4635,28 +4635,28 @@
         <v>0</v>
       </c>
       <c r="Z33" t="n">
-        <v>323.33</v>
+        <v>768.98</v>
       </c>
       <c r="AA33" t="n">
-        <v>101.79</v>
+        <v>279.25</v>
       </c>
       <c r="AB33" t="n">
         <v>0</v>
       </c>
       <c r="AC33" t="n">
-        <v>101.79</v>
+        <v>279.25</v>
       </c>
       <c r="AD33" t="n">
         <v>0</v>
       </c>
       <c r="AE33" t="n">
-        <v>61.65</v>
+        <v>53.07</v>
       </c>
       <c r="AF33" t="n">
         <v>0</v>
       </c>
       <c r="AG33" t="n">
-        <v>38.35</v>
+        <v>46.93</v>
       </c>
       <c r="AH33" t="inlineStr">
         <is>
@@ -4685,30 +4685,30 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Havlíčkova 68, 269 01 Rakovník</t>
+          <t>ČEZ Energo, s.r.o., Kotelská 9027, 337 01 Rokycany</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>27ZG200Z02360612</t>
+          <t>27ZG300Z0249752G</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>796</v>
+        <v>2733</v>
       </c>
       <c r="F34" t="n">
-        <v>796</v>
+        <v>2733</v>
       </c>
       <c r="G34" t="n">
-        <v>29995</v>
+        <v>153043</v>
       </c>
       <c r="H34" t="n">
-        <v>65590</v>
+        <v>585163</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
@@ -4720,7 +4720,7 @@
         <v>0</v>
       </c>
       <c r="L34" t="n">
-        <v>796</v>
+        <v>2733</v>
       </c>
       <c r="M34" t="n">
         <v>0</v>
@@ -4732,13 +4732,13 @@
         <v>0</v>
       </c>
       <c r="P34" t="n">
-        <v>65590</v>
+        <v>585163</v>
       </c>
       <c r="Q34" t="n">
         <v>0</v>
       </c>
       <c r="R34" t="n">
-        <v>221.11</v>
+        <v>759.17</v>
       </c>
       <c r="S34" t="n">
         <v>0</v>
@@ -4750,10 +4750,10 @@
         <v>0</v>
       </c>
       <c r="V34" t="n">
-        <v>221.11</v>
+        <v>759.17</v>
       </c>
       <c r="W34" t="n">
-        <v>221.11</v>
+        <v>759.17</v>
       </c>
       <c r="X34" t="n">
         <v>0</v>
@@ -4762,28 +4762,28 @@
         <v>0</v>
       </c>
       <c r="Z34" t="n">
-        <v>329.39</v>
+        <v>1668.17</v>
       </c>
       <c r="AA34" t="n">
-        <v>65.59</v>
+        <v>585.16</v>
       </c>
       <c r="AB34" t="n">
         <v>0</v>
       </c>
       <c r="AC34" t="n">
-        <v>65.59</v>
+        <v>585.16</v>
       </c>
       <c r="AD34" t="n">
         <v>0</v>
       </c>
       <c r="AE34" t="n">
-        <v>77.12</v>
+        <v>56.47</v>
       </c>
       <c r="AF34" t="n">
         <v>0</v>
       </c>
       <c r="AG34" t="n">
-        <v>22.88</v>
+        <v>43.53</v>
       </c>
       <c r="AH34" t="inlineStr">
         <is>
@@ -4812,30 +4812,30 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., Na Pátku 881, 337 01 Rokycany</t>
+          <t>ČEZ Energo, s.r.o., Havlíčkova 68, 269 01 Rakovník</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>27ZG300Z0249631S</t>
+          <t>27ZG200Z02360612</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>238</v>
+        <v>3418</v>
       </c>
       <c r="F35" t="n">
-        <v>238</v>
+        <v>3418</v>
       </c>
       <c r="G35" t="n">
-        <v>6043</v>
+        <v>157667</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>457130</v>
       </c>
       <c r="I35" t="n">
         <v>0</v>
@@ -4847,7 +4847,7 @@
         <v>0</v>
       </c>
       <c r="L35" t="n">
-        <v>238</v>
+        <v>3418</v>
       </c>
       <c r="M35" t="n">
         <v>0</v>
@@ -4859,13 +4859,13 @@
         <v>0</v>
       </c>
       <c r="P35" t="n">
-        <v>0</v>
+        <v>457130</v>
       </c>
       <c r="Q35" t="n">
         <v>0</v>
       </c>
       <c r="R35" t="n">
-        <v>66.11</v>
+        <v>949.4400000000001</v>
       </c>
       <c r="S35" t="n">
         <v>0</v>
@@ -4877,10 +4877,10 @@
         <v>0</v>
       </c>
       <c r="V35" t="n">
-        <v>66.11</v>
+        <v>949.4400000000001</v>
       </c>
       <c r="W35" t="n">
-        <v>66.11</v>
+        <v>949.4400000000001</v>
       </c>
       <c r="X35" t="n">
         <v>0</v>
@@ -4889,32 +4889,32 @@
         <v>0</v>
       </c>
       <c r="Z35" t="n">
-        <v>66.36</v>
+        <v>1718.57</v>
       </c>
       <c r="AA35" t="n">
-        <v>0</v>
+        <v>457.13</v>
       </c>
       <c r="AB35" t="n">
         <v>0</v>
       </c>
       <c r="AC35" t="n">
-        <v>0</v>
+        <v>457.13</v>
       </c>
       <c r="AD35" t="n">
         <v>0</v>
       </c>
       <c r="AE35" t="n">
-        <v>100</v>
+        <v>67.5</v>
       </c>
       <c r="AF35" t="n">
         <v>0</v>
       </c>
       <c r="AG35" t="n">
-        <v>0</v>
+        <v>32.5</v>
       </c>
       <c r="AH35" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t>ANO</t>
         </is>
       </c>
       <c r="AI35" t="inlineStr">
@@ -4939,30 +4939,30 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., U Teplárny 617, Česká Třebová</t>
+          <t>ČEZ Energo, s.r.o., Na Pátku 881, 337 01 Rokycany</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>27ZG500Z0292262E</t>
+          <t>27ZG300Z0249631S</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>136.91</v>
+        <v>1127</v>
       </c>
       <c r="F36" t="n">
-        <v>136.91</v>
+        <v>1127</v>
       </c>
       <c r="G36" t="n">
-        <v>3647.36</v>
+        <v>57048</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>180289</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
@@ -4974,10 +4974,10 @@
         <v>0</v>
       </c>
       <c r="L36" t="n">
-        <v>0</v>
+        <v>1127</v>
       </c>
       <c r="M36" t="n">
-        <v>136.91</v>
+        <v>0</v>
       </c>
       <c r="N36" t="n">
         <v>0</v>
@@ -4986,13 +4986,13 @@
         <v>0</v>
       </c>
       <c r="P36" t="n">
-        <v>0</v>
+        <v>180289</v>
       </c>
       <c r="Q36" t="n">
         <v>0</v>
       </c>
       <c r="R36" t="n">
-        <v>38.03</v>
+        <v>313.06</v>
       </c>
       <c r="S36" t="n">
         <v>0</v>
@@ -5004,59 +5004,59 @@
         <v>0</v>
       </c>
       <c r="V36" t="n">
-        <v>38.03</v>
+        <v>313.06</v>
       </c>
       <c r="W36" t="n">
-        <v>0</v>
+        <v>313.06</v>
       </c>
       <c r="X36" t="n">
-        <v>38.03</v>
+        <v>0</v>
       </c>
       <c r="Y36" t="n">
         <v>0</v>
       </c>
       <c r="Z36" t="n">
-        <v>40.03</v>
+        <v>621.8200000000001</v>
       </c>
       <c r="AA36" t="n">
-        <v>0</v>
+        <v>180.29</v>
       </c>
       <c r="AB36" t="n">
         <v>0</v>
       </c>
       <c r="AC36" t="n">
-        <v>0</v>
+        <v>180.29</v>
       </c>
       <c r="AD36" t="n">
         <v>0</v>
       </c>
       <c r="AE36" t="n">
-        <v>0</v>
+        <v>63.46</v>
       </c>
       <c r="AF36" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AG36" t="n">
-        <v>0</v>
+        <v>36.54</v>
       </c>
       <c r="AH36" t="inlineStr">
         <is>
+          <t>ANO</t>
+        </is>
+      </c>
+      <c r="AI36" t="inlineStr">
+        <is>
           <t>NE</t>
         </is>
       </c>
-      <c r="AI36" t="inlineStr">
-        <is>
-          <t>NE</t>
-        </is>
-      </c>
       <c r="AJ36" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t>ANO</t>
         </is>
       </c>
       <c r="AK36" t="inlineStr">
         <is>
-          <t>Z1</t>
+          <t>O</t>
         </is>
       </c>
     </row>
@@ -5066,30 +5066,30 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ČEZ Energo, s.r.o., 24, Klimkovice, 742 83</t>
+          <t>ČEZ Energo, s.r.o., U Teplárny 617, Česká Třebová</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Srpen</t>
+          <t>Prosinec</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>27ZG700Z0000506T</t>
+          <t>27ZG500Z0292262E</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>924.6</v>
+        <v>423.02</v>
       </c>
       <c r="F37" t="n">
-        <v>924.6</v>
+        <v>423.02</v>
       </c>
       <c r="G37" t="n">
-        <v>42556</v>
+        <v>11347.68</v>
       </c>
       <c r="H37" t="n">
-        <v>118600</v>
+        <v>0</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
@@ -5104,7 +5104,7 @@
         <v>0</v>
       </c>
       <c r="M37" t="n">
-        <v>924.6</v>
+        <v>423.02</v>
       </c>
       <c r="N37" t="n">
         <v>0</v>
@@ -5113,13 +5113,13 @@
         <v>0</v>
       </c>
       <c r="P37" t="n">
-        <v>118600</v>
+        <v>0</v>
       </c>
       <c r="Q37" t="n">
         <v>0</v>
       </c>
       <c r="R37" t="n">
-        <v>256.83</v>
+        <v>117.51</v>
       </c>
       <c r="S37" t="n">
         <v>0</v>
@@ -5131,28 +5131,28 @@
         <v>0</v>
       </c>
       <c r="V37" t="n">
-        <v>256.83</v>
+        <v>117.51</v>
       </c>
       <c r="W37" t="n">
         <v>0</v>
       </c>
       <c r="X37" t="n">
-        <v>256.83</v>
+        <v>117.51</v>
       </c>
       <c r="Y37" t="n">
         <v>0</v>
       </c>
       <c r="Z37" t="n">
-        <v>466.8</v>
+        <v>123.69</v>
       </c>
       <c r="AA37" t="n">
-        <v>118.6</v>
+        <v>0</v>
       </c>
       <c r="AB37" t="n">
         <v>0</v>
       </c>
       <c r="AC37" t="n">
-        <v>118.6</v>
+        <v>0</v>
       </c>
       <c r="AD37" t="n">
         <v>0</v>
@@ -5161,10 +5161,10 @@
         <v>0</v>
       </c>
       <c r="AF37" t="n">
-        <v>68.41</v>
+        <v>100</v>
       </c>
       <c r="AG37" t="n">
-        <v>31.59</v>
+        <v>0</v>
       </c>
       <c r="AH37" t="inlineStr">
         <is>
@@ -5193,122 +5193,249 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
+          <t>ČEZ Energo, s.r.o., 24, Klimkovice, 742 83</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Prosinec</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>27ZG700Z0000506T</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>2577.09</v>
+      </c>
+      <c r="F38" t="n">
+        <v>2577.09</v>
+      </c>
+      <c r="G38" t="n">
+        <v>122969</v>
+      </c>
+      <c r="H38" t="n">
+        <v>379040</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" t="n">
+        <v>2577.09</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" t="n">
+        <v>379040</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" t="n">
+        <v>715.86</v>
+      </c>
+      <c r="S38" t="n">
+        <v>0</v>
+      </c>
+      <c r="T38" t="n">
+        <v>0</v>
+      </c>
+      <c r="U38" t="n">
+        <v>0</v>
+      </c>
+      <c r="V38" t="n">
+        <v>715.86</v>
+      </c>
+      <c r="W38" t="n">
+        <v>0</v>
+      </c>
+      <c r="X38" t="n">
+        <v>715.86</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>1340.36</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>379.04</v>
+      </c>
+      <c r="AB38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC38" t="n">
+        <v>379.04</v>
+      </c>
+      <c r="AD38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF38" t="n">
+        <v>65.38</v>
+      </c>
+      <c r="AG38" t="n">
+        <v>34.62</v>
+      </c>
+      <c r="AH38" t="inlineStr">
+        <is>
+          <t>ANO</t>
+        </is>
+      </c>
+      <c r="AI38" t="inlineStr">
+        <is>
+          <t>NE</t>
+        </is>
+      </c>
+      <c r="AJ38" t="inlineStr">
+        <is>
+          <t>NE</t>
+        </is>
+      </c>
+      <c r="AK38" t="inlineStr">
+        <is>
+          <t>Z1</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
           <t>ČEZ Energo, s.r.o., TeVi,Výstavní 1144/103, 703 00 Ostrava-Vítkovice</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Srpen</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Prosinec</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
         <is>
           <t>27ZG705Z0000037P</t>
         </is>
       </c>
-      <c r="E38" t="n">
-        <v>4245</v>
-      </c>
-      <c r="F38" t="n">
-        <v>4270</v>
-      </c>
-      <c r="G38" t="n">
-        <v>257432</v>
-      </c>
-      <c r="H38" t="n">
-        <v>1024242</v>
-      </c>
-      <c r="I38" t="n">
-        <v>0</v>
-      </c>
-      <c r="J38" t="n">
-        <v>-25</v>
-      </c>
-      <c r="K38" t="n">
-        <v>0</v>
-      </c>
-      <c r="L38" t="n">
-        <v>4270</v>
-      </c>
-      <c r="M38" t="n">
-        <v>0</v>
-      </c>
-      <c r="N38" t="n">
-        <v>0</v>
-      </c>
-      <c r="O38" t="n">
-        <v>0</v>
-      </c>
-      <c r="P38" t="n">
-        <v>1024242</v>
-      </c>
-      <c r="Q38" t="n">
-        <v>0</v>
-      </c>
-      <c r="R38" t="n">
-        <v>1179.17</v>
-      </c>
-      <c r="S38" t="n">
-        <v>0</v>
-      </c>
-      <c r="T38" t="n">
-        <v>-6.94</v>
-      </c>
-      <c r="U38" t="n">
-        <v>0</v>
-      </c>
-      <c r="V38" t="n">
-        <v>1186.11</v>
-      </c>
-      <c r="W38" t="n">
-        <v>1186.11</v>
-      </c>
-      <c r="X38" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y38" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z38" t="n">
-        <v>2823.8</v>
-      </c>
-      <c r="AA38" t="n">
-        <v>1024.24</v>
-      </c>
-      <c r="AB38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC38" t="n">
-        <v>1024.24</v>
-      </c>
-      <c r="AD38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE38" t="n">
-        <v>53.52</v>
-      </c>
-      <c r="AF38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG38" t="n">
-        <v>46.48</v>
-      </c>
-      <c r="AH38" t="inlineStr">
-        <is>
-          <t>ANO</t>
-        </is>
-      </c>
-      <c r="AI38" t="inlineStr">
+      <c r="E39" t="n">
+        <v>4050</v>
+      </c>
+      <c r="F39" t="n">
+        <v>4049</v>
+      </c>
+      <c r="G39" t="n">
+        <v>252036</v>
+      </c>
+      <c r="H39" t="n">
+        <v>972868</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>1</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" t="n">
+        <v>4049</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" t="n">
+        <v>0</v>
+      </c>
+      <c r="P39" t="n">
+        <v>972868</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" t="n">
+        <v>1125</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0</v>
+      </c>
+      <c r="T39" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="U39" t="n">
+        <v>0</v>
+      </c>
+      <c r="V39" t="n">
+        <v>1124.72</v>
+      </c>
+      <c r="W39" t="n">
+        <v>1124.72</v>
+      </c>
+      <c r="X39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>2747.19</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>972.87</v>
+      </c>
+      <c r="AB39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC39" t="n">
+        <v>972.87</v>
+      </c>
+      <c r="AD39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE39" t="n">
+        <v>53.63</v>
+      </c>
+      <c r="AF39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG39" t="n">
+        <v>46.37</v>
+      </c>
+      <c r="AH39" t="inlineStr">
+        <is>
+          <t>ANO</t>
+        </is>
+      </c>
+      <c r="AI39" t="inlineStr">
         <is>
           <t>NE</t>
         </is>
       </c>
-      <c r="AJ38" t="inlineStr">
-        <is>
-          <t>ANO</t>
-        </is>
-      </c>
-      <c r="AK38" t="inlineStr">
+      <c r="AJ39" t="inlineStr">
+        <is>
+          <t>ANO</t>
+        </is>
+      </c>
+      <c r="AK39" t="inlineStr">
         <is>
           <t>O</t>
         </is>

</xml_diff>